<commit_message>
ASLDRO-103: changed gradient echo equation
Gradient echo mri signal model now uses the equation which allows
arbitrary flip angles.
</commit_message>
<xml_diff>
--- a/src/asldro/data/mri_signal_validation_calculations.xlsx
+++ b/src/asldro/data/mri_signal_validation_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7930D409-E0B5-4C12-B384-369E71C6709F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA8D75B-72B1-4C86-9602-870AEF64BFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>MRI signal model validation calculator</t>
   </si>
@@ -68,13 +68,25 @@
   <si>
     <t>Spin Echo</t>
   </si>
+  <si>
+    <t>flip_angle</t>
+  </si>
+  <si>
+    <t>echo_time</t>
+  </si>
+  <si>
+    <t>repetition_time</t>
+  </si>
+  <si>
+    <t>flip_angle_radians</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.00000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -107,7 +119,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -248,42 +260,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>GE!$G$6:$G$16</c:f>
+              <c:f>GE!$I$6:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00000000000E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.51045834044304694</c:v>
+                  <c:v>0.51046968571193507</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44250505407323171</c:v>
+                  <c:v>0.44251488903609754</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38359785190384371</c:v>
+                  <c:v>0.38360637761579697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33253250020708525</c:v>
+                  <c:v>0.33253989095835718</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2882650753781949</c:v>
+                  <c:v>0.28827148225713506</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24989062311517735</c:v>
+                  <c:v>0.24989617709693698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.21662465853334917</c:v>
+                  <c:v>0.2166294731573922</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.18778712902348998</c:v>
+                  <c:v>0.18779130271466848</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16278851200799938</c:v>
+                  <c:v>0.16279213008864241</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14111776339295173</c:v>
+                  <c:v>0.14112089982710069</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.12233187034752503</c:v>
+                  <c:v>0.12233458925297279</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1962,16 +1974,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2305,35 +2317,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="2" customWidth="1"/>
     <col min="2" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2347,16 +2361,22 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1.4</v>
       </c>
@@ -2375,12 +2395,19 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
-        <f>C6*(1-EXP(-F6/A6))*EXP(-E6/D6)</f>
-        <v>0.51045834044304694</v>
+      <c r="G6" s="2">
+        <v>90</v>
+      </c>
+      <c r="H6" s="2">
+        <f>RADIANS(G6)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I6" s="1">
+        <f>SIN(H6)*C6*(1-EXP(-F6/A6))/(1-COS(H6)*EXP(-F6/A6)-EXP(-F6/B6)*(EXP(-F6/A6)-COS(H6)))*EXP(-E6/D6)</f>
+        <v>0.51046968571193507</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1.4</v>
       </c>
@@ -2399,12 +2426,19 @@
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
-        <f>C7*(1-EXP(-F7/A7))*EXP(-E7/D7)</f>
-        <v>0.44250505407323171</v>
+      <c r="G7" s="2">
+        <v>90</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H16" si="0">RADIANS(G7)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:I16" si="1">SIN(H7)*C7*(1-EXP(-F7/A7))/(1-COS(H7)*EXP(-F7/A7)-EXP(-F7/B7)*(EXP(-F7/A7)-COS(H7)))*EXP(-E7/D7)</f>
+        <v>0.44251488903609754</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1.4</v>
       </c>
@@ -2423,12 +2457,19 @@
       <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="1">
-        <f t="shared" ref="G8:G16" si="0">C8*(1-EXP(-F8/A8))*EXP(-E8/D8)</f>
-        <v>0.38359785190384371</v>
+      <c r="G8" s="2">
+        <v>90</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38360637761579697</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1.4</v>
       </c>
@@ -2447,12 +2488,19 @@
       <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
+        <v>90</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>0.33253250020708525</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33253989095835718</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1.4</v>
       </c>
@@ -2471,12 +2519,19 @@
       <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
+        <v>90</v>
+      </c>
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>0.2882650753781949</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28827148225713506</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1.4</v>
       </c>
@@ -2495,12 +2550,19 @@
       <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
+        <v>90</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>0.24989062311517735</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24989617709693698</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1.4</v>
       </c>
@@ -2519,12 +2581,19 @@
       <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
+        <v>90</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>0.21662465853334917</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2166294731573922</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1.4</v>
       </c>
@@ -2543,12 +2612,19 @@
       <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
+        <v>90</v>
+      </c>
+      <c r="H13" s="2">
         <f t="shared" si="0"/>
-        <v>0.18778712902348998</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.18779130271466848</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1.4</v>
       </c>
@@ -2567,12 +2643,19 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
+        <v>90</v>
+      </c>
+      <c r="H14" s="2">
         <f t="shared" si="0"/>
-        <v>0.16278851200799938</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16279213008864241</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1.4</v>
       </c>
@@ -2591,12 +2674,19 @@
       <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
+        <v>90</v>
+      </c>
+      <c r="H15" s="2">
         <f t="shared" si="0"/>
-        <v>0.14111776339295173</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14112089982710069</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1.4</v>
       </c>
@@ -2615,9 +2705,16 @@
       <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
+        <v>90</v>
+      </c>
+      <c r="H16" s="2">
         <f t="shared" si="0"/>
-        <v>0.12233187034752503</v>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12233458925297279</v>
       </c>
     </row>
   </sheetData>
@@ -2630,7 +2727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB82AFF-2AFC-46C7-851A-E8E5AB55514C}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ASLDRO-103: Added inversion recovery mri model
</commit_message>
<xml_diff>
--- a/src/asldro/data/mri_signal_validation_calculations.xlsx
+++ b/src/asldro/data/mri_signal_validation_calculations.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aaron\Seafile\aot_code\python\asldro\src\asldro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA8D75B-72B1-4C86-9602-870AEF64BFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9084C3AC-093F-45DC-99EB-B1B2EA5DE8B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE" sheetId="1" r:id="rId1"/>
     <sheet name="SE" sheetId="2" r:id="rId2"/>
+    <sheet name="IR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>MRI signal model validation calculator</t>
   </si>
@@ -80,13 +81,26 @@
   <si>
     <t>flip_angle_radians</t>
   </si>
+  <si>
+    <t>Inversion Recovery</t>
+  </si>
+  <si>
+    <t>inversion_angle</t>
+  </si>
+  <si>
+    <t>inversion_angle_radians</t>
+  </si>
+  <si>
+    <t>inversion_time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.00000000000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -117,10 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,6 +873,371 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IR!$K$6:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IR!$L$6:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000000E+00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>-0.90412215281300534</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.77936819997462892</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.66321443786586565</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.55506799324380074</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.45437686389887372</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.3606271011194489</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.27334018638944468</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.19207058892913903</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.11640349161231978</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.5952673652387366E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9641460749809481E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4718622331716778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.69324314058920644</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.80161831740060752</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85467248131163909</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8806447047590521</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.89335919012788256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.89958346039575254</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5418-4332-961B-83C1667B8332}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="375555952"/>
+        <c:axId val="717041648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="375555952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="717041648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="717041648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00000000000000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375555952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -938,6 +1318,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1455,6 +1875,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2032,6 +2968,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC590A1-9023-463B-9104-206AB0290C4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7098883-1D1D-483D-B458-8C9903A2BB7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2319,7 +3298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6:I16"/>
     </sheetView>
   </sheetViews>
@@ -3044,4 +4023,819 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB498D3-A8BF-44F7-A847-050C3FA0AAA4}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="2" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="17.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2">
+        <v>90</v>
+      </c>
+      <c r="H6" s="2">
+        <f>RADIANS(G6)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I6" s="2">
+        <v>180</v>
+      </c>
+      <c r="J6" s="2">
+        <f>RADIANS(I6)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <f>(C6*(1- (1 -COS(J6)) * EXP(-K6 / A6)- COS(J6) * EXP(-F6 / A6))/ (1- COS(H6)* COS(J6)* EXP(-F6 / A6)))* EXP(-E6 / B6)</f>
+        <v>-0.90412215281300534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <v>90</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H16" si="0">RADIANS(G7)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I7" s="2">
+        <v>180</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" ref="J7:J23" si="1">RADIANS(I7)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" ref="L7:L16" si="2">(C7*(1- (1 -COS(J7)) * EXP(-K7 / A7)- COS(J7) * EXP(-F7 / A7))/ (1- COS(H7)* COS(J7)* EXP(-F7 / A7)))* EXP(-E7 / B7)</f>
+        <v>-0.77936819997462892</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>90</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I8" s="2">
+        <v>180</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.66321443786586565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>90</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I9" s="2">
+        <v>180</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.55506799324380074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="2">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2">
+        <v>90</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I10" s="2">
+        <v>180</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.45437686389887372</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2">
+        <v>90</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I11" s="2">
+        <v>180</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.3606271011194489</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2">
+        <v>90</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I12" s="2">
+        <v>180</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.27334018638944468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <v>90</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I13" s="2">
+        <v>180</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.19207058892913903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F14" s="2">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2">
+        <v>90</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I14" s="2">
+        <v>180</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.11640349161231978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F15" s="2">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2">
+        <v>90</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I15" s="2">
+        <v>180</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.5952673652387366E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>90</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I16" s="2">
+        <v>180</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.9641460749809481E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="2">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2">
+        <v>90</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" ref="H17" si="3">RADIANS(G17)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I17" s="2">
+        <v>180</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" ref="L17" si="4">(C17*(1- (1 -COS(J17)) * EXP(-K17 / A17)- COS(J17) * EXP(-F17 / A17))/ (1- COS(H17)* COS(J17)* EXP(-F17 / A17)))* EXP(-E17 / B17)</f>
+        <v>0.4718622331716778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F18" s="2">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2">
+        <v>90</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18:H23" si="5">RADIANS(G18)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I18" s="2">
+        <v>180</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" ref="L18:L23" si="6">(C18*(1- (1 -COS(J18)) * EXP(-K18 / A18)- COS(J18) * EXP(-F18 / A18))/ (1- COS(H18)* COS(J18)* EXP(-F18 / A18)))* EXP(-E18 / B18)</f>
+        <v>0.69324314058920644</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="2">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2">
+        <v>90</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I19" s="2">
+        <v>180</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="6"/>
+        <v>0.80161831740060752</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F20" s="2">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2">
+        <v>90</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I20" s="2">
+        <v>180</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K20" s="2">
+        <v>5</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="6"/>
+        <v>0.85467248131163909</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F21" s="2">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2">
+        <v>90</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I21" s="2">
+        <v>180</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K21" s="2">
+        <v>6</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="6"/>
+        <v>0.8806447047590521</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2">
+        <v>90</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I22" s="2">
+        <v>180</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K22" s="2">
+        <v>7</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="6"/>
+        <v>0.89335919012788256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F23" s="2">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2">
+        <v>90</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I23" s="2">
+        <v>180</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K23" s="2">
+        <v>8</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="6"/>
+        <v>0.89958346039575254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>